<commit_message>
This is new update1.1
</commit_message>
<xml_diff>
--- a/тесткейс01.xlsx
+++ b/тесткейс01.xlsx
@@ -14,17 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Action(действия)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Expected result(ожидаемый результат)</t>
   </si>
   <si>
-    <t>Test result</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -40,7 +34,72 @@
     <t>Открыть страницу "Вход в систему"</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Окно "Вход в систему" открыто            2. Название окна "Вход в систему"           3. Логотип компании отображается в правом верхнем углу                                            4. На форме 2 поля "Имя" и "Пароль"     5. Кнопка Вход доступна                                6. Ссылка "забыть пароль" доступна       </t>
+    <t>Тест отправки комментария</t>
+  </si>
+  <si>
+    <t>Action(действия)/Steps</t>
+  </si>
+  <si>
+    <t>Test result/Factual result</t>
+  </si>
+  <si>
+    <t>"Тип обращения"-Комментарий
+"Контактное лицо"- Ангелина
+"E-mail"- anglenich@mail.ru
+"Сообщение"- Добрый день, уважаемые пользователи данного сайта!
+Хочу поздравить всех с предстоящими 
+праздниками и пожелать всем добра и
+счастья! Уважайте друг друга)</t>
+  </si>
+  <si>
+    <t>1. Заполнить форму 
+отправки комментрая
+2. Нажать на кнопку "Отправить"</t>
+  </si>
+  <si>
+    <t>"E-mail"- anglenich@mail.ru
+"Password"-angela1919</t>
+  </si>
+  <si>
+    <t>1. Открыть  сайт Ситилинк
+https://www.citilink.ru/
+2. Перейти по сыллке 
+с названием "Задать впорос" 
+внизу страницы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Открыть  сайт Ситилинк
+https://www.citilink.ru/
+2. Пользователь должен быть уже зарегистрирован в системе
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Окно "Вход в систему" открыто            2. Название окна "Вход в систему"           3. Логотип компании отображается в правом верхнем углу                                            4. На форме 2 поля "Email" и "Пароль"     5. Кнопка Вход доступна
+6. Пользователя впустило в систему                                
+7. Ссылка "забыть пароль" доступна       </t>
+  </si>
+  <si>
+    <t>1. Нажать на кнопку "Войти" 
+в правой части сайта
+2.Ввести Email и пароль
+в поля ввода
+3. Нажать на кнопку "Войти"</t>
+  </si>
+  <si>
+    <t>1. Сайт Про тестинг открыт и доступен
+2. Страница "Вопросы, пожелания и заявки" открыта и доступна
+3. Данные успешно введены
+4. Комментарий успешно отправлен
+5. Страница "Ваш запрос успешно отправлен!" открыта</t>
+  </si>
+  <si>
+    <t>Пользователя впустило в 
+систему 
+Тест прошел - passed</t>
+  </si>
+  <si>
+    <t>Запрос успешно отправлен
+Тест прошел - passed</t>
   </si>
 </sst>
 </file>
@@ -56,12 +115,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -76,13 +141,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -388,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,50 +473,86 @@
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="F3" s="2"/>
     </row>
+    <row r="4" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>